<commit_message>
issues with calculating mean - symp leg vs asymp leg
</commit_message>
<xml_diff>
--- a/SLDJ_Input.xlsx
+++ b/SLDJ_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Subject</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Trial Limb</t>
+  </si>
+  <si>
+    <t>First VFrame</t>
+  </si>
+  <si>
+    <t>Last VFrame</t>
   </si>
   <si>
     <t>File Path</t>
@@ -404,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,125 +437,167 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>415</v>
+      </c>
+      <c r="G2">
+        <v>477</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>503</v>
+      </c>
+      <c r="G3">
+        <v>578</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>376</v>
+      </c>
+      <c r="G4">
+        <v>452</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>232</v>
+      </c>
+      <c r="G5">
+        <v>295</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>345</v>
+      </c>
+      <c r="G6">
+        <v>410</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>